<commit_message>
finish system_utils.py of utils
</commit_message>
<xml_diff>
--- a/assets/results_1102.xlsx
+++ b/assets/results_1102.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23145" windowHeight="9555" activeTab="1"/>
+    <workbookView windowWidth="23145" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="Nerf-Synthetic" sheetId="1" r:id="rId1"/>
@@ -1289,8 +1289,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J250"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="59" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -8179,8 +8179,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView zoomScale="58" zoomScaleNormal="58" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>

</xml_diff>